<commit_message>
filling db and any commands
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\All\School_web\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEF38F8-1F6E-416B-80C8-B85CFCB8EC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0800D4-56E1-403A-A554-301C55BB4E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10400" activeTab="1" xr2:uid="{AF44F801-155E-4DF1-8B43-AC8FD0A461BD}"/>
+    <workbookView xWindow="-4510" yWindow="1570" windowWidth="9470" windowHeight="8300" activeTab="1" xr2:uid="{AF44F801-155E-4DF1-8B43-AC8FD0A461BD}"/>
   </bookViews>
   <sheets>
     <sheet name="RU" sheetId="1" r:id="rId1"/>
@@ -633,6 +633,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,12 +673,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1011,12 +1011,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -1058,16 +1058,16 @@
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:15" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -1122,18 +1122,18 @@
       <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:15" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -1150,7 +1150,7 @@
       <c r="C12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="23" t="s">
         <v>59</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -1225,16 +1225,16 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:15" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
@@ -1299,7 +1299,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1318,12 +1318,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -1365,16 +1365,16 @@
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:13" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -1424,18 +1424,18 @@
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:13" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
@@ -1447,7 +1447,7 @@
       <c r="C12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -1504,16 +1504,16 @@
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>

</xml_diff>